<commit_message>
After 2nd round of selection for drug-like set.
</commit_message>
<xml_diff>
--- a/compound_selection/zinc15_eMolecules_intersection_set/20170807_zinc15_eMolecules_subset_depiction/df_drug_final_oe.xlsx
+++ b/compound_selection/zinc15_eMolecules_intersection_set/20170807_zinc15_eMolecules_subset_depiction/df_drug_final_oe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="105">
   <si>
     <t>df_drug_final_oe.csv</t>
   </si>
@@ -64,16 +64,16 @@
     <t>canonical isomeric SMILES</t>
   </si>
   <si>
-    <t>[3.523, 7.492]</t>
-  </si>
-  <si>
-    <t>3.253999948501587</t>
-  </si>
-  <si>
-    <t>400.473</t>
-  </si>
-  <si>
-    <t>110.0</t>
+    <t>[3.511, 6.794]</t>
+  </si>
+  <si>
+    <t>3.370999813079834</t>
+  </si>
+  <si>
+    <t>396.95099999999996</t>
+  </si>
+  <si>
+    <t>239.0</t>
   </si>
   <si>
     <t>168.0</t>
@@ -82,241 +82,247 @@
     <t>drug-like</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>picked</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Ic1cc(I)c2c(c1O)nccc2</t>
+  </si>
+  <si>
+    <t>c1cc2c(cc(c(c2nc1)O)I)I</t>
+  </si>
+  <si>
+    <t>[6.336]</t>
+  </si>
+  <si>
+    <t>2.937000036239624</t>
+  </si>
+  <si>
+    <t>420.461</t>
+  </si>
+  <si>
+    <t>319.0</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>CCOC(=O)c1ccc(cc1)Nc1cc(C)nc(n1)Nc1ccc(cc1)C(=O)OCC</t>
+  </si>
+  <si>
+    <t>CCOC(=O)c1ccc(cc1)Nc2cc(nc(n2)Nc3ccc(cc3)C(=O)OCC)C</t>
+  </si>
+  <si>
+    <t>[9.381, 10.773]</t>
+  </si>
+  <si>
+    <t>3.3410000801086426</t>
+  </si>
+  <si>
+    <t>426.439</t>
+  </si>
+  <si>
+    <t>247.7</t>
+  </si>
+  <si>
+    <t>223.0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>O=C(Nc1ncc(s1)Cc1ccc(c(c1)F)F)CCc1nc2ccccc2c(=O)[nH]1</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(=O)[nH]c(n2)CCC(=O)Nc3ncc(s3)Cc4ccc(c(c4)F)F</t>
+  </si>
+  <si>
+    <t>[3.892]</t>
+  </si>
+  <si>
+    <t>4.140000343322754</t>
+  </si>
+  <si>
+    <t>438.092</t>
+  </si>
+  <si>
+    <t>222.0</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Brc1cccc(c1)Nc1ncc(c(n1)Nc1cccc(c1)Br)F</t>
+  </si>
+  <si>
+    <t>c1cc(cc(c1)Br)Nc2c(cnc(n2)Nc3cccc(c3)Br)F</t>
+  </si>
+  <si>
+    <t>[9.167]</t>
+  </si>
+  <si>
+    <t>5.171000480651856</t>
+  </si>
+  <si>
+    <t>381.276</t>
+  </si>
+  <si>
+    <t>489.9</t>
+  </si>
+  <si>
+    <t>148.0</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>CCOc1ccc2c(c1)sc(n2)NC(=O)Cc1ccc(c(c1)Cl)Cl</t>
+  </si>
+  <si>
+    <t>CCOc1ccc2c(c1)sc(n2)NC(=O)Cc3ccc(c(c3)Cl)Cl</t>
+  </si>
+  <si>
+    <t>[8.05]</t>
+  </si>
+  <si>
+    <t>5.238000392913818</t>
+  </si>
+  <si>
+    <t>380.245</t>
+  </si>
+  <si>
+    <t>154.0</t>
+  </si>
+  <si>
+    <t>219.0</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>O=C1NC(=O)/C(=C\c2cccc(c2)OCc2ccc(cc2Cl)Cl)/S1</t>
+  </si>
+  <si>
+    <t>c1cc(cc(c1)OCc2ccc(cc2Cl)Cl)/C=C/3\C(=O)NC(=O)S3</t>
+  </si>
+  <si>
+    <t>[3.199]</t>
+  </si>
+  <si>
+    <t>4.7179999351501465</t>
+  </si>
+  <si>
+    <t>401.481</t>
+  </si>
+  <si>
+    <t>636.9</t>
+  </si>
+  <si>
+    <t>249.0</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>O=C(c1ccccc1)Nc1ccc(cc1)Oc1ncnc2c1c1CCCCc1s2</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)C(=O)Nc2ccc(cc2)Oc3c4c5c(sc4ncn3)CCCC5</t>
+  </si>
+  <si>
+    <t>[4.113]</t>
+  </si>
+  <si>
+    <t>5.7840003967285165</t>
+  </si>
+  <si>
+    <t>403.305</t>
+  </si>
+  <si>
+    <t>324.5</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>O=C(Nc1cccc(c1Cl)Cl)Nc1cc(nn1c1ccccc1)C(C)(C)C</t>
+  </si>
+  <si>
+    <t>CC(C)(C)c1cc(n(n1)c2ccccc2)NC(=O)Nc3cccc(c3Cl)Cl</t>
+  </si>
+  <si>
+    <t>[6.525]</t>
+  </si>
+  <si>
+    <t>5.9000000953674325</t>
+  </si>
+  <si>
+    <t>440.765</t>
+  </si>
+  <si>
+    <t>239.5</t>
+  </si>
+  <si>
+    <t>400.0</t>
+  </si>
+  <si>
+    <t>Brc1ccc(cc1)CSc1nnc(s1)NC(=O)c1ccccc1Cl</t>
+  </si>
+  <si>
+    <t>c1ccc(c(c1)C(=O)Nc2nnc(s2)SCc3ccc(cc3)Br)Cl</t>
+  </si>
+  <si>
+    <t>[4.829]</t>
+  </si>
+  <si>
+    <t>2.7940003871917725</t>
+  </si>
+  <si>
+    <t>391.42</t>
+  </si>
+  <si>
+    <t>398.0</t>
+  </si>
+  <si>
     <t>71</t>
-  </si>
-  <si>
-    <t>picked</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>O1CCN(CC1)CCNc1ncnc2c1c(c1ccccc1)c(o2)c1ccccc1</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)c2c3c(ncnc3oc2c4ccccc4)NCCN5CCOCC5</t>
-  </si>
-  <si>
-    <t>[6.336]</t>
-  </si>
-  <si>
-    <t>2.937000036239624</t>
-  </si>
-  <si>
-    <t>420.461</t>
-  </si>
-  <si>
-    <t>319.0</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>CCOC(=O)c1ccc(cc1)Nc1cc(C)nc(n1)Nc1ccc(cc1)C(=O)OCC</t>
-  </si>
-  <si>
-    <t>CCOC(=O)c1ccc(cc1)Nc2cc(nc(n2)Nc3ccc(cc3)C(=O)OCC)C</t>
-  </si>
-  <si>
-    <t>[9.381, 10.773]</t>
-  </si>
-  <si>
-    <t>3.3410000801086426</t>
-  </si>
-  <si>
-    <t>426.439</t>
-  </si>
-  <si>
-    <t>247.7</t>
-  </si>
-  <si>
-    <t>223.0</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>O=C(Nc1ncc(s1)Cc1ccc(c(c1)F)F)CCc1nc2ccccc2c(=O)[nH]1</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)c(=O)[nH]c(n2)CCC(=O)Nc3ncc(s3)Cc4ccc(c(c4)F)F</t>
-  </si>
-  <si>
-    <t>[3.892]</t>
-  </si>
-  <si>
-    <t>4.140000343322754</t>
-  </si>
-  <si>
-    <t>438.092</t>
-  </si>
-  <si>
-    <t>222.0</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>Brc1cccc(c1)Nc1ncc(c(n1)Nc1cccc(c1)Br)F</t>
-  </si>
-  <si>
-    <t>c1cc(cc(c1)Br)Nc2c(cnc(n2)Nc3cccc(c3)Br)F</t>
-  </si>
-  <si>
-    <t>[9.167]</t>
-  </si>
-  <si>
-    <t>5.171000480651856</t>
-  </si>
-  <si>
-    <t>381.276</t>
-  </si>
-  <si>
-    <t>489.9</t>
-  </si>
-  <si>
-    <t>148.0</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>CCOc1ccc2c(c1)sc(n2)NC(=O)Cc1ccc(c(c1)Cl)Cl</t>
-  </si>
-  <si>
-    <t>CCOc1ccc2c(c1)sc(n2)NC(=O)Cc3ccc(c(c3)Cl)Cl</t>
-  </si>
-  <si>
-    <t>[8.05]</t>
-  </si>
-  <si>
-    <t>5.238000392913818</t>
-  </si>
-  <si>
-    <t>380.245</t>
-  </si>
-  <si>
-    <t>154.0</t>
-  </si>
-  <si>
-    <t>219.0</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>O=C1NC(=O)/C(=C\c2cccc(c2)OCc2ccc(cc2Cl)Cl)/S1</t>
-  </si>
-  <si>
-    <t>c1cc(cc(c1)OCc2ccc(cc2Cl)Cl)/C=C/3\C(=O)NC(=O)S3</t>
-  </si>
-  <si>
-    <t>[3.199]</t>
-  </si>
-  <si>
-    <t>4.7179999351501465</t>
-  </si>
-  <si>
-    <t>401.481</t>
-  </si>
-  <si>
-    <t>636.9</t>
-  </si>
-  <si>
-    <t>249.0</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>O=C(c1ccccc1)Nc1ccc(cc1)Oc1ncnc2c1c1CCCCc1s2</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)C(=O)Nc2ccc(cc2)Oc3c4c5c(sc4ncn3)CCCC5</t>
-  </si>
-  <si>
-    <t>[4.113]</t>
-  </si>
-  <si>
-    <t>5.7840003967285165</t>
-  </si>
-  <si>
-    <t>403.305</t>
-  </si>
-  <si>
-    <t>324.5</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>4.0</t>
-  </si>
-  <si>
-    <t>O=C(Nc1cccc(c1Cl)Cl)Nc1cc(nn1c1ccccc1)C(C)(C)C</t>
-  </si>
-  <si>
-    <t>CC(C)(C)c1cc(n(n1)c2ccccc2)NC(=O)Nc3cccc(c3Cl)Cl</t>
-  </si>
-  <si>
-    <t>[6.525]</t>
-  </si>
-  <si>
-    <t>5.9000000953674325</t>
-  </si>
-  <si>
-    <t>440.765</t>
-  </si>
-  <si>
-    <t>239.5</t>
-  </si>
-  <si>
-    <t>400.0</t>
-  </si>
-  <si>
-    <t>Brc1ccc(cc1)CSc1nnc(s1)NC(=O)c1ccccc1Cl</t>
-  </si>
-  <si>
-    <t>c1ccc(c(c1)C(=O)Nc2nnc(s2)SCc3ccc(cc3)Br)Cl</t>
-  </si>
-  <si>
-    <t>[4.829]</t>
-  </si>
-  <si>
-    <t>2.7940003871917725</t>
-  </si>
-  <si>
-    <t>391.42</t>
-  </si>
-  <si>
-    <t>398.0</t>
   </si>
   <si>
     <t>OCCNc1ncnc2c1c(c1ccc(cc1)OC)c(o2)c1ccc(cc1)OC</t>
@@ -1105,7 +1111,7 @@
     <col min="1" max="1" width="38.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
@@ -1335,7 +1341,7 @@
         <v>54</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>27</v>
@@ -1367,7 +1373,7 @@
         <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>35</v>
@@ -1376,36 +1382,36 @@
         <v>24</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>21</v>
@@ -1414,57 +1420,57 @@
         <v>53</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>36</v>
@@ -1473,24 +1479,24 @@
         <v>27</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B10" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>61</v>
@@ -1499,86 +1505,86 @@
         <v>21</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B12" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>20</v>
@@ -1590,22 +1596,22 @@
         <v>44</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>